<commit_message>
BolusDosage Preprocessing + mat files
</commit_message>
<xml_diff>
--- a/data_analysis/PythonPipeline/Modules/Patient_9_SBS_Scores.xlsx
+++ b/data_analysis/PythonPipeline/Modules/Patient_9_SBS_Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b14a0d7b62cf6ad0/Sid Stuff/PROJECTS/iMEDS Design Team/Data Analysis/PedAccel/data_analysis/PythonPipeline/Modules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{A015547E-2BDB-4BC4-98C3-3AFEEE514619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55EC7627-D7B7-4C46-ACAE-136914B587D7}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{A015547E-2BDB-4BC4-98C3-3AFEEE514619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65635EDB-6FAD-4F1A-ADB7-E673296D6F61}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{809031ED-8969-471B-B3A5-4615F6501142}"/>
   </bookViews>
@@ -664,7 +664,7 @@
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>